<commit_message>
Automação do Google concluida
</commit_message>
<xml_diff>
--- a/Trabalho/Colegio_Madre_Cabrini/new_matricula.xlsx
+++ b/Trabalho/Colegio_Madre_Cabrini/new_matricula.xlsx
@@ -36,12 +36,6 @@
     <t>Data_de_Nascimento</t>
   </si>
   <si>
-    <t>Geovane Santos Bussola teste1</t>
-  </si>
-  <si>
-    <t>Evandro David teste2</t>
-  </si>
-  <si>
     <t>Turma</t>
   </si>
   <si>
@@ -198,7 +192,13 @@
     <t>3-m-b</t>
   </si>
   <si>
-    <t>Fernada Ferreira Souza teste3</t>
+    <t>teste teste teste2</t>
+  </si>
+  <si>
+    <t>teste teste teste1</t>
+  </si>
+  <si>
+    <t>teste teste teste3</t>
   </si>
 </sst>
 </file>
@@ -543,7 +543,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,12 +565,12 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>56</v>
       </c>
       <c r="B2" s="1">
         <v>50014001</v>
@@ -579,12 +579,12 @@
         <v>39109</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>55</v>
       </c>
       <c r="B3" s="1">
         <v>50014002</v>
@@ -593,7 +593,7 @@
         <v>36556</v>
       </c>
       <c r="D3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -607,7 +607,7 @@
         <v>36568</v>
       </c>
       <c r="D4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -648,257 +648,257 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Criação da automação do moodle
</commit_message>
<xml_diff>
--- a/Trabalho/Colegio_Madre_Cabrini/new_matricula.xlsx
+++ b/Trabalho/Colegio_Madre_Cabrini/new_matricula.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="57">
   <si>
     <t>Nome</t>
   </si>
@@ -193,9 +193,6 @@
   </si>
   <si>
     <t>teste teste teste2</t>
-  </si>
-  <si>
-    <t>teste teste teste1</t>
   </si>
   <si>
     <t>teste teste teste3</t>
@@ -543,7 +540,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,43 +567,29 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B2" s="1">
-        <v>50014001</v>
+        <v>50014002</v>
       </c>
       <c r="C2" s="5">
-        <v>39109</v>
+        <v>36556</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B3" s="1">
-        <v>50014002</v>
+        <v>50014003</v>
       </c>
       <c r="C3" s="5">
-        <v>36556</v>
+        <v>36568</v>
       </c>
       <c r="D3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B4" s="1">
-        <v>50014003</v>
-      </c>
-      <c r="C4" s="5">
-        <v>36568</v>
-      </c>
-      <c r="D4" t="s">
         <v>53</v>
       </c>
     </row>
@@ -628,7 +611,7 @@
           <x14:formula1>
             <xm:f>Planilha2!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D496</xm:sqref>
+          <xm:sqref>D2:D3 D5:D496</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Goodle e Moodle prontos
</commit_message>
<xml_diff>
--- a/Trabalho/Colegio_Madre_Cabrini/new_matricula.xlsx
+++ b/Trabalho/Colegio_Madre_Cabrini/new_matricula.xlsx
@@ -543,7 +543,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,7 +579,7 @@
         <v>36556</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -593,7 +593,7 @@
         <v>36597</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -607,7 +607,7 @@
         <v>36721</v>
       </c>
       <c r="D4" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Automação da Iônica completa
</commit_message>
<xml_diff>
--- a/Trabalho/Colegio_Madre_Cabrini/new_matricula.xlsx
+++ b/Trabalho/Colegio_Madre_Cabrini/new_matricula.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2160" windowHeight="0"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="2160" windowHeight="0"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -543,7 +543,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,7 +579,7 @@
         <v>36556</v>
       </c>
       <c r="D2" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>